<commit_message>
VS as absolute value and redo
</commit_message>
<xml_diff>
--- a/masterdata.xlsx
+++ b/masterdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simba/Dharma/Ideas&amp;Projects/Academic/Projects/Dairy_Agroecosystems/Analysis/GitHub/DairyEffluents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9060DC2F-976B-6644-B890-7144706E1FF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36FA07F-E049-004C-9C1F-2D65EDACFA24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MasterData" sheetId="9" r:id="rId1"/>
@@ -586,7 +586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -595,9 +595,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -921,10 +918,10 @@
   <dimension ref="A1:AP97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C79" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F55" sqref="F55"/>
+      <selection pane="bottomRight" activeCell="AM7" sqref="AM7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -934,137 +931,137 @@
     <col min="4" max="4" width="11.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="35" width="10.83203125" style="3"/>
     <col min="36" max="36" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.33203125" style="3" customWidth="1"/>
     <col min="38" max="38" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="39" max="42" width="10.83203125" style="2"/>
     <col min="43" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="15" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:42" s="14" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="N1" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="O1" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="P1" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="Q1" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="R1" s="15" t="s">
+      <c r="R1" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="S1" s="15" t="s">
+      <c r="S1" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="T1" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="U1" s="15" t="s">
+      <c r="U1" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="V1" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="W1" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="X1" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="Y1" s="15" t="s">
+      <c r="Y1" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="Z1" s="15" t="s">
+      <c r="Z1" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="AA1" s="15" t="s">
+      <c r="AA1" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="AB1" s="15" t="s">
+      <c r="AB1" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="AC1" s="15" t="s">
+      <c r="AC1" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="AD1" s="15" t="s">
+      <c r="AD1" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="AE1" s="15" t="s">
+      <c r="AE1" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="AF1" s="15" t="s">
+      <c r="AF1" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="AG1" s="15" t="s">
+      <c r="AG1" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="AH1" s="15" t="s">
+      <c r="AH1" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="AI1" s="15" t="s">
+      <c r="AI1" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="AJ1" s="15" t="s">
+      <c r="AJ1" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="AK1" s="15" t="s">
+      <c r="AK1" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="AL1" s="8" t="s">
+      <c r="AL1" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="AM1" s="8" t="s">
+      <c r="AM1" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="AN1" s="8" t="s">
+      <c r="AN1" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="AO1" s="8" t="s">
+      <c r="AO1" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="AP1" s="15" t="s">
+      <c r="AP1" s="14" t="s">
         <v>136</v>
       </c>
     </row>
@@ -1087,7 +1084,7 @@
       <c r="F2" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <v>43899</v>
       </c>
       <c r="H2" s="1">
@@ -1184,8 +1181,8 @@
       <c r="AJ2" s="1">
         <v>4.690831556503201</v>
       </c>
-      <c r="AK2" s="4">
-        <v>67.045454545454675</v>
+      <c r="AK2" s="1">
+        <v>3.1449893390191979</v>
       </c>
       <c r="AL2" s="2">
         <v>100</v>
@@ -1196,7 +1193,7 @@
       <c r="AN2" s="2">
         <v>110</v>
       </c>
-      <c r="AO2" s="9">
+      <c r="AO2" s="8">
         <v>0</v>
       </c>
       <c r="AP2" s="2">
@@ -1223,7 +1220,7 @@
       <c r="F3" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>43899</v>
       </c>
       <c r="H3" s="1">
@@ -1320,8 +1317,8 @@
       <c r="AJ3" s="1">
         <v>1.7457180500659024</v>
       </c>
-      <c r="AK3" s="4">
-        <v>62.26415094339427</v>
+      <c r="AK3" s="1">
+        <v>1.0869565217391126</v>
       </c>
       <c r="AL3" s="2">
         <v>80</v>
@@ -1332,7 +1329,7 @@
       <c r="AN3" s="2">
         <v>80</v>
       </c>
-      <c r="AO3" s="9">
+      <c r="AO3" s="8">
         <v>0</v>
       </c>
       <c r="AP3" s="2">
@@ -1359,7 +1356,7 @@
       <c r="F4" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>43899</v>
       </c>
       <c r="H4" s="1">
@@ -1456,17 +1453,17 @@
       <c r="AJ4" s="1">
         <v>15.526675786593733</v>
       </c>
-      <c r="AK4" s="4">
-        <v>53.30396475770938</v>
-      </c>
-      <c r="AL4" s="10">
+      <c r="AK4" s="1">
+        <v>8.2763337893297191</v>
+      </c>
+      <c r="AL4" s="9">
         <v>16</v>
       </c>
-      <c r="AM4" s="10">
+      <c r="AM4" s="9">
         <v>20</v>
       </c>
-      <c r="AN4" s="11"/>
-      <c r="AO4" s="11"/>
+      <c r="AN4" s="10"/>
+      <c r="AO4" s="10"/>
       <c r="AP4" s="2">
         <f t="shared" si="6"/>
         <v>18</v>
@@ -1491,7 +1488,7 @@
       <c r="F5" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>43899</v>
       </c>
       <c r="H5" s="1">
@@ -1588,8 +1585,8 @@
       <c r="AJ5" s="1">
         <v>0.58981233243968467</v>
       </c>
-      <c r="AK5" s="4">
-        <v>54.545454545456018</v>
+      <c r="AK5" s="1">
+        <v>0.32171581769438212</v>
       </c>
       <c r="AL5" s="2">
         <v>100</v>
@@ -1600,7 +1597,7 @@
       <c r="AN5" s="2">
         <v>120</v>
       </c>
-      <c r="AO5" s="9">
+      <c r="AO5" s="8">
         <v>0</v>
       </c>
       <c r="AP5" s="2">
@@ -1621,13 +1618,13 @@
       <c r="D6" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="16" t="s">
         <v>138</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>43906</v>
       </c>
       <c r="H6" s="1">
@@ -1724,8 +1721,8 @@
       <c r="AJ6" s="1">
         <v>0.87615439261188532</v>
       </c>
-      <c r="AK6" s="4">
-        <v>62.162162162161451</v>
+      <c r="AK6" s="1">
+        <v>0.54463651432630089</v>
       </c>
       <c r="AL6" s="2">
         <v>50</v>
@@ -1736,7 +1733,7 @@
       <c r="AN6" s="2">
         <v>60</v>
       </c>
-      <c r="AO6" s="9">
+      <c r="AO6" s="8">
         <v>0</v>
       </c>
       <c r="AP6" s="2">
@@ -1757,13 +1754,13 @@
       <c r="D7" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="17" t="s">
         <v>139</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>43906</v>
       </c>
       <c r="H7" s="1">
@@ -1860,8 +1857,8 @@
       <c r="AJ7" s="1">
         <v>1.0425020048115754</v>
       </c>
-      <c r="AK7" s="4">
-        <v>38.461538461540037</v>
+      <c r="AK7" s="1">
+        <v>0.40096230954293005</v>
       </c>
       <c r="AL7" s="2">
         <v>110</v>
@@ -1872,7 +1869,7 @@
       <c r="AN7" s="2">
         <v>100</v>
       </c>
-      <c r="AO7" s="9">
+      <c r="AO7" s="8">
         <v>0</v>
       </c>
       <c r="AP7" s="2">
@@ -1893,13 +1890,13 @@
       <c r="D8" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="17" t="s">
         <v>140</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>43906</v>
       </c>
       <c r="H8" s="1">
@@ -1996,17 +1993,17 @@
       <c r="AJ8" s="1">
         <v>25.389408099688499</v>
       </c>
-      <c r="AK8" s="4">
-        <v>88.343558282208534</v>
-      </c>
-      <c r="AL8" s="12">
+      <c r="AK8" s="1">
+        <v>22.429906542056084</v>
+      </c>
+      <c r="AL8" s="11">
         <v>29</v>
       </c>
-      <c r="AM8" s="12">
+      <c r="AM8" s="11">
         <v>35</v>
       </c>
-      <c r="AN8" s="11"/>
-      <c r="AO8" s="11"/>
+      <c r="AN8" s="10"/>
+      <c r="AO8" s="10"/>
       <c r="AP8" s="2">
         <f t="shared" si="6"/>
         <v>32</v>
@@ -2025,13 +2022,13 @@
       <c r="D9" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="17" t="s">
         <v>141</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>43906</v>
       </c>
       <c r="H9" s="1">
@@ -2128,19 +2125,19 @@
       <c r="AJ9" s="1">
         <v>0.6192660550458543</v>
       </c>
-      <c r="AK9" s="4">
-        <v>29.629629629627193</v>
+      <c r="AK9" s="1">
+        <v>0.18348623853208987</v>
       </c>
       <c r="AL9" s="2">
         <v>100</v>
       </c>
-      <c r="AM9" s="13">
+      <c r="AM9" s="12">
         <v>0</v>
       </c>
       <c r="AN9" s="2">
         <v>90</v>
       </c>
-      <c r="AO9" s="13">
+      <c r="AO9" s="12">
         <v>0</v>
       </c>
       <c r="AP9" s="2">
@@ -2167,7 +2164,7 @@
       <c r="F10" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>43977</v>
       </c>
       <c r="H10" s="1">
@@ -2264,19 +2261,19 @@
       <c r="AJ10" s="1">
         <v>2.933333333333306</v>
       </c>
-      <c r="AK10" s="4">
-        <v>14.772727272727296</v>
+      <c r="AK10" s="1">
+        <v>0.43333333333333002</v>
       </c>
       <c r="AL10" s="2">
         <v>60</v>
       </c>
-      <c r="AM10" s="13">
+      <c r="AM10" s="12">
         <v>0</v>
       </c>
       <c r="AN10" s="2">
         <v>50</v>
       </c>
-      <c r="AO10" s="13">
+      <c r="AO10" s="12">
         <v>0</v>
       </c>
       <c r="AP10" s="2">
@@ -2303,7 +2300,7 @@
       <c r="F11" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <v>43977</v>
       </c>
       <c r="H11" s="1">
@@ -2400,8 +2397,8 @@
       <c r="AJ11" s="1">
         <v>2.9315960912052068</v>
       </c>
-      <c r="AK11" s="4">
-        <v>24.444444444444752</v>
+      <c r="AK11" s="1">
+        <v>0.71661237785017062</v>
       </c>
       <c r="AL11" s="2">
         <v>1000</v>
@@ -2439,7 +2436,7 @@
       <c r="F12" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <v>43977</v>
       </c>
       <c r="H12" s="1">
@@ -2536,17 +2533,17 @@
       <c r="AJ12" s="1">
         <v>25.131578947368521</v>
       </c>
-      <c r="AK12" s="4">
-        <v>90.052356020942383</v>
-      </c>
-      <c r="AL12" s="12">
+      <c r="AK12" s="1">
+        <v>22.631578947368503</v>
+      </c>
+      <c r="AL12" s="11">
         <v>40</v>
       </c>
-      <c r="AM12" s="12">
+      <c r="AM12" s="11">
         <v>40</v>
       </c>
-      <c r="AN12" s="11"/>
-      <c r="AO12" s="11"/>
+      <c r="AN12" s="10"/>
+      <c r="AO12" s="10"/>
       <c r="AP12" s="2">
         <f t="shared" si="6"/>
         <v>40</v>
@@ -2571,7 +2568,7 @@
       <c r="F13" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <v>43977</v>
       </c>
       <c r="H13" s="1">
@@ -2668,19 +2665,19 @@
       <c r="AJ13" s="1">
         <v>3.1111111111111303</v>
       </c>
-      <c r="AK13" s="4">
-        <v>11.904761904762635</v>
+      <c r="AK13" s="1">
+        <v>0.37037037037039539</v>
       </c>
       <c r="AL13" s="2">
         <v>60</v>
       </c>
-      <c r="AM13" s="13">
+      <c r="AM13" s="12">
         <v>0</v>
       </c>
       <c r="AN13" s="2">
         <v>100</v>
       </c>
-      <c r="AO13" s="13">
+      <c r="AO13" s="12">
         <v>0</v>
       </c>
       <c r="AP13" s="2">
@@ -2701,13 +2698,13 @@
       <c r="D14" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E14" s="16" t="s">
         <v>138</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <v>43979</v>
       </c>
       <c r="H14" s="1">
@@ -2804,8 +2801,8 @@
       <c r="AJ14" s="1">
         <v>2.0000000000000169</v>
       </c>
-      <c r="AK14" s="4">
-        <v>21.66666666666632</v>
+      <c r="AK14" s="1">
+        <v>0.43333333333333002</v>
       </c>
       <c r="AL14" s="2">
         <v>1200</v>
@@ -2837,13 +2834,13 @@
       <c r="D15" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="17" t="s">
         <v>139</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
         <v>43979</v>
       </c>
       <c r="H15" s="1">
@@ -2940,8 +2937,8 @@
       <c r="AJ15" s="1">
         <v>2.8124999999999947</v>
       </c>
-      <c r="AK15" s="4">
-        <v>21.111111111109313</v>
+      <c r="AK15" s="1">
+        <v>0.59374999999994826</v>
       </c>
       <c r="AL15" s="2">
         <v>1200</v>
@@ -2973,13 +2970,13 @@
       <c r="D16" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="17" t="s">
         <v>140</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="4">
         <v>43979</v>
       </c>
       <c r="H16" s="1">
@@ -3076,17 +3073,17 @@
       <c r="AJ16" s="1">
         <v>19.915966386554622</v>
       </c>
-      <c r="AK16" s="4">
-        <v>32.489451476793221</v>
-      </c>
-      <c r="AL16" s="12">
+      <c r="AK16" s="1">
+        <v>6.4705882352941124</v>
+      </c>
+      <c r="AL16" s="11">
         <v>88</v>
       </c>
-      <c r="AM16" s="12">
+      <c r="AM16" s="11">
         <v>100</v>
       </c>
-      <c r="AN16" s="11"/>
-      <c r="AO16" s="11"/>
+      <c r="AN16" s="10"/>
+      <c r="AO16" s="10"/>
       <c r="AP16" s="2">
         <f t="shared" si="6"/>
         <v>94</v>
@@ -3105,13 +3102,13 @@
       <c r="D17" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="17" t="s">
         <v>141</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="4">
         <v>43979</v>
       </c>
       <c r="H17" s="1">
@@ -3208,8 +3205,8 @@
       <c r="AJ17" s="1">
         <v>0.52083333333332227</v>
       </c>
-      <c r="AK17" s="4">
-        <v>15.000000000000888</v>
+      <c r="AK17" s="1">
+        <v>7.812500000000297E-2</v>
       </c>
       <c r="AL17" s="2">
         <v>190</v>
@@ -3220,7 +3217,7 @@
       <c r="AN17" s="2">
         <v>220</v>
       </c>
-      <c r="AO17" s="13">
+      <c r="AO17" s="12">
         <v>0</v>
       </c>
       <c r="AP17" s="2">
@@ -3247,7 +3244,7 @@
       <c r="F18" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="4">
         <v>43983</v>
       </c>
       <c r="H18" s="1">
@@ -3344,8 +3341,8 @@
       <c r="AJ18" s="1">
         <v>2.000000000000016</v>
       </c>
-      <c r="AK18" s="4">
-        <v>26.666666666666472</v>
+      <c r="AK18" s="1">
+        <v>0.53333333333333366</v>
       </c>
       <c r="AL18" s="2">
         <v>2400</v>
@@ -3383,7 +3380,7 @@
       <c r="F19" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="4">
         <v>43983</v>
       </c>
       <c r="H19" s="1">
@@ -3480,8 +3477,8 @@
       <c r="AJ19" s="1">
         <v>3.7617554858934197</v>
       </c>
-      <c r="AK19" s="4">
-        <v>17.499999999999908</v>
+      <c r="AK19" s="1">
+        <v>0.65830721003134496</v>
       </c>
       <c r="AL19" s="2">
         <v>2000</v>
@@ -3519,7 +3516,7 @@
       <c r="F20" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="4">
         <v>43983</v>
       </c>
       <c r="H20" s="1">
@@ -3616,17 +3613,17 @@
       <c r="AJ20" s="1">
         <v>29.807692307692378</v>
       </c>
-      <c r="AK20" s="4">
-        <v>85.806451612903089</v>
-      </c>
-      <c r="AL20" s="12">
+      <c r="AK20" s="1">
+        <v>25.576923076923094</v>
+      </c>
+      <c r="AL20" s="11">
         <v>176</v>
       </c>
-      <c r="AM20" s="12">
+      <c r="AM20" s="11">
         <v>188</v>
       </c>
-      <c r="AN20" s="11"/>
-      <c r="AO20" s="11"/>
+      <c r="AN20" s="10"/>
+      <c r="AO20" s="10"/>
       <c r="AP20" s="2">
         <f t="shared" si="6"/>
         <v>182</v>
@@ -3651,7 +3648,7 @@
       <c r="F21" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="4">
         <v>43983</v>
       </c>
       <c r="H21" s="1">
@@ -3748,8 +3745,8 @@
       <c r="AJ21" s="1">
         <v>1.612903225806446</v>
       </c>
-      <c r="AK21" s="4">
-        <v>60.000000000000711</v>
+      <c r="AK21" s="1">
+        <v>0.96774193548387899</v>
       </c>
       <c r="AL21" s="2">
         <v>110</v>
@@ -3760,7 +3757,7 @@
       <c r="AN21" s="2">
         <v>110</v>
       </c>
-      <c r="AO21" s="13">
+      <c r="AO21" s="12">
         <v>0</v>
       </c>
       <c r="AP21" s="2">
@@ -3781,13 +3778,13 @@
       <c r="D22" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E22" s="17" t="s">
+      <c r="E22" s="16" t="s">
         <v>138</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="4">
         <v>43987</v>
       </c>
       <c r="H22" s="1">
@@ -3884,8 +3881,8 @@
       <c r="AJ22" s="1">
         <v>2.2641509433961793</v>
       </c>
-      <c r="AK22" s="4">
-        <v>21.2</v>
+      <c r="AK22" s="1">
+        <v>0.47999999999998999</v>
       </c>
       <c r="AL22" s="2">
         <v>1200</v>
@@ -3917,13 +3914,13 @@
       <c r="D23" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="17" t="s">
         <v>139</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="4">
         <v>43987</v>
       </c>
       <c r="H23" s="1">
@@ -4020,8 +4017,8 @@
       <c r="AJ23" s="1">
         <v>2.7586206896551744</v>
       </c>
-      <c r="AK23" s="4">
-        <v>24.999999999999446</v>
+      <c r="AK23" s="1">
+        <v>0.68965517241377827</v>
       </c>
       <c r="AL23" s="2">
         <v>800</v>
@@ -4053,13 +4050,13 @@
       <c r="D24" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="17" t="s">
         <v>140</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="4">
         <v>43987</v>
       </c>
       <c r="H24" s="1">
@@ -4156,17 +4153,17 @@
       <c r="AJ24" s="1">
         <v>32.352941176470523</v>
       </c>
-      <c r="AK24" s="4">
-        <v>77.272727272727323</v>
-      </c>
-      <c r="AL24" s="12">
+      <c r="AK24" s="1">
+        <v>24.999999999999968</v>
+      </c>
+      <c r="AL24" s="11">
         <v>240</v>
       </c>
-      <c r="AM24" s="12">
+      <c r="AM24" s="11">
         <v>240</v>
       </c>
-      <c r="AN24" s="11"/>
-      <c r="AO24" s="11"/>
+      <c r="AN24" s="10"/>
+      <c r="AO24" s="10"/>
       <c r="AP24" s="2">
         <f t="shared" si="6"/>
         <v>240</v>
@@ -4185,13 +4182,13 @@
       <c r="D25" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="17" t="s">
         <v>141</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="4">
         <v>43987</v>
       </c>
       <c r="H25" s="1">
@@ -4288,19 +4285,19 @@
       <c r="AJ25" s="1">
         <v>2.6666666666666683</v>
       </c>
-      <c r="AK25" s="4">
-        <v>20</v>
+      <c r="AK25" s="1">
+        <v>0.53333333333333366</v>
       </c>
       <c r="AL25" s="2">
         <v>150</v>
       </c>
-      <c r="AM25" s="13">
+      <c r="AM25" s="12">
         <v>0</v>
       </c>
       <c r="AN25" s="2">
         <v>150</v>
       </c>
-      <c r="AO25" s="13">
+      <c r="AO25" s="12">
         <v>0</v>
       </c>
       <c r="AP25" s="2">
@@ -4327,7 +4324,7 @@
       <c r="F26" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="4">
         <v>43991</v>
       </c>
       <c r="H26" s="1">
@@ -4421,7 +4418,7 @@
         <f t="shared" si="5"/>
         <v>1.0999999999999999</v>
       </c>
-      <c r="AJ26" s="6"/>
+      <c r="AJ26" s="5"/>
       <c r="AK26" s="6"/>
       <c r="AL26" s="2">
         <v>2000</v>
@@ -4459,7 +4456,7 @@
       <c r="F27" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27" s="4">
         <v>43991</v>
       </c>
       <c r="H27" s="1">
@@ -4553,7 +4550,7 @@
         <f t="shared" si="5"/>
         <v>1.2000000000000002</v>
       </c>
-      <c r="AJ27" s="6"/>
+      <c r="AJ27" s="5"/>
       <c r="AK27" s="6"/>
       <c r="AL27" s="2">
         <v>1440</v>
@@ -4591,7 +4588,7 @@
       <c r="F28" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="4">
         <v>43991</v>
       </c>
       <c r="H28" s="1">
@@ -4685,16 +4682,16 @@
         <f t="shared" si="5"/>
         <v>1.2</v>
       </c>
-      <c r="AJ28" s="6"/>
+      <c r="AJ28" s="5"/>
       <c r="AK28" s="6"/>
-      <c r="AL28" s="12">
+      <c r="AL28" s="11">
         <v>260</v>
       </c>
-      <c r="AM28" s="12">
+      <c r="AM28" s="11">
         <v>284</v>
       </c>
-      <c r="AN28" s="11"/>
-      <c r="AO28" s="11"/>
+      <c r="AN28" s="10"/>
+      <c r="AO28" s="10"/>
       <c r="AP28" s="2">
         <f t="shared" si="6"/>
         <v>272</v>
@@ -4719,7 +4716,7 @@
       <c r="F29" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="4">
         <v>43991</v>
       </c>
       <c r="H29" s="1">
@@ -4813,7 +4810,7 @@
         <f t="shared" si="5"/>
         <v>1.04</v>
       </c>
-      <c r="AJ29" s="6"/>
+      <c r="AJ29" s="5"/>
       <c r="AK29" s="6"/>
       <c r="AL29" s="2">
         <v>300</v>
@@ -4845,13 +4842,13 @@
       <c r="D30" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="16" t="s">
         <v>138</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G30" s="4">
         <v>43994</v>
       </c>
       <c r="H30" s="1">
@@ -4948,8 +4945,8 @@
       <c r="AJ30" s="1">
         <v>0.74324324324325119</v>
       </c>
-      <c r="AK30" s="4">
-        <v>40.909090909092008</v>
+      <c r="AK30" s="1">
+        <v>0.30405405405406549</v>
       </c>
       <c r="AL30" s="2">
         <v>1400</v>
@@ -4981,13 +4978,13 @@
       <c r="D31" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E31" s="18" t="s">
+      <c r="E31" s="17" t="s">
         <v>139</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G31" s="5">
+      <c r="G31" s="4">
         <v>43994</v>
       </c>
       <c r="H31" s="1">
@@ -5084,8 +5081,8 @@
       <c r="AJ31" s="1">
         <v>0.82706766917291907</v>
       </c>
-      <c r="AK31" s="4">
-        <v>39.393939393939718</v>
+      <c r="AK31" s="1">
+        <v>0.32581453634084956</v>
       </c>
       <c r="AL31" s="2">
         <v>1280</v>
@@ -5117,13 +5114,13 @@
       <c r="D32" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E32" s="18" t="s">
+      <c r="E32" s="17" t="s">
         <v>140</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G32" s="4">
         <v>43994</v>
       </c>
       <c r="H32" s="1">
@@ -5220,17 +5217,17 @@
       <c r="AJ32" s="1">
         <v>27.663384064458441</v>
       </c>
-      <c r="AK32" s="4">
-        <v>88.025889967637312</v>
-      </c>
-      <c r="AL32" s="12">
+      <c r="AK32" s="1">
+        <v>24.350940017905099</v>
+      </c>
+      <c r="AL32" s="11">
         <v>140</v>
       </c>
-      <c r="AM32" s="12">
+      <c r="AM32" s="11">
         <v>156</v>
       </c>
-      <c r="AN32" s="11"/>
-      <c r="AO32" s="11"/>
+      <c r="AN32" s="10"/>
+      <c r="AO32" s="10"/>
       <c r="AP32" s="2">
         <f t="shared" si="6"/>
         <v>148</v>
@@ -5249,13 +5246,13 @@
       <c r="D33" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E33" s="18" t="s">
+      <c r="E33" s="17" t="s">
         <v>141</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G33" s="5">
+      <c r="G33" s="4">
         <v>43994</v>
       </c>
       <c r="H33" s="1">
@@ -5352,8 +5349,8 @@
       <c r="AJ33" s="1">
         <v>0.37288135593220745</v>
       </c>
-      <c r="AK33" s="4">
-        <v>46.33</v>
+      <c r="AK33" s="1">
+        <v>0.17275593220339172</v>
       </c>
       <c r="AL33" s="2">
         <v>120</v>
@@ -5391,7 +5388,7 @@
       <c r="F34" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G34" s="5">
+      <c r="G34" s="4">
         <v>43998</v>
       </c>
       <c r="H34" s="1">
@@ -5488,8 +5485,8 @@
       <c r="AJ34" s="1">
         <v>0.88957055214723668</v>
       </c>
-      <c r="AK34" s="4">
-        <v>3.1034482758609707</v>
+      <c r="AK34" s="1">
+        <v>2.7607361963180335E-2</v>
       </c>
       <c r="AL34" s="2">
         <v>1640</v>
@@ -5527,7 +5524,7 @@
       <c r="F35" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G35" s="5">
+      <c r="G35" s="4">
         <v>43998</v>
       </c>
       <c r="H35" s="1">
@@ -5624,8 +5621,8 @@
       <c r="AJ35" s="1">
         <v>1.8298261665141691</v>
       </c>
-      <c r="AK35" s="4">
-        <v>11.666666666666197</v>
+      <c r="AK35" s="1">
+        <v>0.21347971942664448</v>
       </c>
       <c r="AL35" s="2">
         <v>800</v>
@@ -5663,7 +5660,7 @@
       <c r="F36" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G36" s="5">
+      <c r="G36" s="4">
         <v>43998</v>
       </c>
       <c r="H36" s="1">
@@ -5760,17 +5757,17 @@
       <c r="AJ36" s="1">
         <v>51.491228070175509</v>
       </c>
-      <c r="AK36" s="4">
-        <v>57.751277683134596</v>
-      </c>
-      <c r="AL36" s="12">
+      <c r="AK36" s="1">
+        <v>29.736842105263204</v>
+      </c>
+      <c r="AL36" s="11">
         <v>280</v>
       </c>
-      <c r="AM36" s="12">
+      <c r="AM36" s="11">
         <v>266</v>
       </c>
-      <c r="AN36" s="11"/>
-      <c r="AO36" s="11"/>
+      <c r="AN36" s="10"/>
+      <c r="AO36" s="10"/>
       <c r="AP36" s="2">
         <f t="shared" si="6"/>
         <v>273</v>
@@ -5795,7 +5792,7 @@
       <c r="F37" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G37" s="4">
         <v>43998</v>
       </c>
       <c r="H37" s="1">
@@ -5892,8 +5889,8 @@
       <c r="AJ37" s="1">
         <v>0.51282051282049657</v>
       </c>
-      <c r="AK37" s="4">
-        <v>46.33</v>
+      <c r="AK37" s="1">
+        <v>0.23758974358973606</v>
       </c>
       <c r="AL37" s="2">
         <v>260</v>
@@ -5925,13 +5922,13 @@
       <c r="D38" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="E38" s="16" t="s">
         <v>138</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G38" s="5">
+      <c r="G38" s="4">
         <v>44000</v>
       </c>
       <c r="H38" s="1">
@@ -6028,19 +6025,19 @@
       <c r="AJ38" s="1">
         <v>0.72420036210015493</v>
       </c>
-      <c r="AK38" s="4">
-        <v>21.3</v>
+      <c r="AK38" s="1">
+        <v>0.15425467712733301</v>
       </c>
       <c r="AL38" s="2">
         <v>2400</v>
       </c>
-      <c r="AM38" s="13">
+      <c r="AM38" s="12">
         <v>0</v>
       </c>
       <c r="AN38" s="2">
         <v>2440</v>
       </c>
-      <c r="AO38" s="13">
+      <c r="AO38" s="12">
         <v>0</v>
       </c>
       <c r="AP38" s="2">
@@ -6061,13 +6058,13 @@
       <c r="D39" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E39" s="18" t="s">
+      <c r="E39" s="17" t="s">
         <v>139</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G39" s="5">
+      <c r="G39" s="4">
         <v>44000</v>
       </c>
       <c r="H39" s="1">
@@ -6164,19 +6161,19 @@
       <c r="AJ39" s="1">
         <v>22.240259740259649</v>
       </c>
-      <c r="AK39" s="4">
-        <v>88.321167883211629</v>
+      <c r="AK39" s="1">
+        <v>19.64285714285705</v>
       </c>
       <c r="AL39" s="2">
         <v>1200</v>
       </c>
-      <c r="AM39" s="13">
+      <c r="AM39" s="12">
         <v>0</v>
       </c>
       <c r="AN39" s="2">
         <v>1250</v>
       </c>
-      <c r="AO39" s="13">
+      <c r="AO39" s="12">
         <v>0</v>
       </c>
       <c r="AP39" s="2">
@@ -6197,13 +6194,13 @@
       <c r="D40" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E40" s="18" t="s">
+      <c r="E40" s="17" t="s">
         <v>140</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G40" s="4">
         <v>44000</v>
       </c>
       <c r="H40" s="1">
@@ -6284,9 +6281,9 @@
         <f t="shared" si="4"/>
         <v>7.2333333333333334</v>
       </c>
-      <c r="AF40" s="7"/>
-      <c r="AG40" s="7"/>
-      <c r="AH40" s="7"/>
+      <c r="AF40" s="6"/>
+      <c r="AG40" s="6"/>
+      <c r="AH40" s="6"/>
       <c r="AI40" s="1" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
@@ -6294,17 +6291,17 @@
       <c r="AJ40" s="1">
         <v>4.4464075382803232</v>
       </c>
-      <c r="AK40" s="4">
-        <v>56.291390728476877</v>
-      </c>
-      <c r="AL40" s="11">
+      <c r="AK40" s="1">
+        <v>2.5029446407538267</v>
+      </c>
+      <c r="AL40" s="10">
         <v>144</v>
       </c>
-      <c r="AM40" s="11">
+      <c r="AM40" s="10">
         <v>160</v>
       </c>
-      <c r="AN40" s="11"/>
-      <c r="AO40" s="11"/>
+      <c r="AN40" s="10"/>
+      <c r="AO40" s="10"/>
       <c r="AP40" s="2">
         <f t="shared" si="6"/>
         <v>152</v>
@@ -6323,13 +6320,13 @@
       <c r="D41" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E41" s="18" t="s">
+      <c r="E41" s="17" t="s">
         <v>141</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G41" s="5">
+      <c r="G41" s="4">
         <v>44000</v>
       </c>
       <c r="H41" s="1">
@@ -6426,19 +6423,19 @@
       <c r="AJ41" s="1">
         <v>10.714285714285653</v>
       </c>
-      <c r="AK41" s="4">
-        <v>83.333333333333584</v>
+      <c r="AK41" s="1">
+        <v>8.9285714285714057</v>
       </c>
       <c r="AL41" s="2">
         <v>1000</v>
       </c>
-      <c r="AM41" s="13">
+      <c r="AM41" s="12">
         <v>0</v>
       </c>
       <c r="AN41" s="2">
         <v>1000</v>
       </c>
-      <c r="AO41" s="13">
+      <c r="AO41" s="12">
         <v>0</v>
       </c>
       <c r="AP41" s="2">
@@ -6465,7 +6462,7 @@
       <c r="F42" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G42" s="5">
+      <c r="G42" s="4">
         <v>44011</v>
       </c>
       <c r="H42" s="1">
@@ -6562,8 +6559,8 @@
       <c r="AJ42" s="1">
         <v>3.0854430379746942</v>
       </c>
-      <c r="AK42" s="4">
-        <v>25.64102564102614</v>
+      <c r="AK42" s="1">
+        <v>0.79113924050634721</v>
       </c>
       <c r="AL42" s="2">
         <v>1000</v>
@@ -6601,7 +6598,7 @@
       <c r="F43" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G43" s="5">
+      <c r="G43" s="4">
         <v>44011</v>
       </c>
       <c r="H43" s="1">
@@ -6698,13 +6695,13 @@
       <c r="AJ43" s="1">
         <v>2.2435897435897454</v>
       </c>
-      <c r="AK43" s="4">
-        <v>35.714285714286511</v>
+      <c r="AK43" s="1">
+        <v>0.80128205128206986</v>
       </c>
       <c r="AL43" s="2">
         <v>750</v>
       </c>
-      <c r="AM43" s="13">
+      <c r="AM43" s="12">
         <v>0</v>
       </c>
       <c r="AN43" s="2">
@@ -6737,7 +6734,7 @@
       <c r="F44" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G44" s="5">
+      <c r="G44" s="4">
         <v>44011</v>
       </c>
       <c r="H44" s="1">
@@ -6834,17 +6831,17 @@
       <c r="AJ44" s="1">
         <v>8.6614173228345805</v>
       </c>
-      <c r="AK44" s="4">
-        <v>45.454545454544906</v>
-      </c>
-      <c r="AL44" s="12">
+      <c r="AK44" s="1">
+        <v>3.9370078740156709</v>
+      </c>
+      <c r="AL44" s="11">
         <v>160</v>
       </c>
-      <c r="AM44" s="12">
+      <c r="AM44" s="11">
         <v>170</v>
       </c>
-      <c r="AN44" s="11"/>
-      <c r="AO44" s="11"/>
+      <c r="AN44" s="10"/>
+      <c r="AO44" s="10"/>
       <c r="AP44" s="2">
         <f t="shared" si="6"/>
         <v>165</v>
@@ -6869,7 +6866,7 @@
       <c r="F45" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G45" s="5">
+      <c r="G45" s="4">
         <v>44011</v>
       </c>
       <c r="H45" s="1">
@@ -6966,13 +6963,13 @@
       <c r="AJ45" s="1">
         <v>6.5180102915951679</v>
       </c>
-      <c r="AK45" s="4">
-        <v>32.894736842104727</v>
+      <c r="AK45" s="1">
+        <v>2.1440823327615335</v>
       </c>
       <c r="AL45" s="2">
         <v>1200</v>
       </c>
-      <c r="AM45" s="13">
+      <c r="AM45" s="12">
         <v>0</v>
       </c>
       <c r="AN45" s="2">
@@ -6999,13 +6996,13 @@
       <c r="D46" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E46" s="17" t="s">
+      <c r="E46" s="16" t="s">
         <v>138</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G46" s="5">
+      <c r="G46" s="4">
         <v>44012</v>
       </c>
       <c r="H46" s="1">
@@ -7102,19 +7099,19 @@
       <c r="AJ46" s="1">
         <v>12.555154432410772</v>
       </c>
-      <c r="AK46" s="4">
-        <v>76.677316293929636</v>
+      <c r="AK46" s="1">
+        <v>9.6269554753309343</v>
       </c>
       <c r="AL46" s="2">
         <v>840</v>
       </c>
-      <c r="AM46" s="13">
+      <c r="AM46" s="12">
         <v>0</v>
       </c>
       <c r="AN46" s="2">
         <v>880</v>
       </c>
-      <c r="AO46" s="13">
+      <c r="AO46" s="12">
         <v>0</v>
       </c>
       <c r="AP46" s="2">
@@ -7135,13 +7132,13 @@
       <c r="D47" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E47" s="18" t="s">
+      <c r="E47" s="17" t="s">
         <v>139</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G47" s="5">
+      <c r="G47" s="4">
         <v>44012</v>
       </c>
       <c r="H47" s="1">
@@ -7238,19 +7235,19 @@
       <c r="AJ47" s="1">
         <v>11.341371514694803</v>
       </c>
-      <c r="AK47" s="4">
-        <v>9.9667774086379524</v>
+      <c r="AK47" s="1">
+        <v>1.1303692539563015</v>
       </c>
       <c r="AL47" s="2">
         <v>2000</v>
       </c>
-      <c r="AM47" s="13">
+      <c r="AM47" s="12">
         <v>0</v>
       </c>
       <c r="AN47" s="2">
         <v>2200</v>
       </c>
-      <c r="AO47" s="13">
+      <c r="AO47" s="12">
         <v>0</v>
       </c>
       <c r="AP47" s="2">
@@ -7271,13 +7268,13 @@
       <c r="D48" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E48" s="18" t="s">
+      <c r="E48" s="17" t="s">
         <v>140</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G48" s="5">
+      <c r="G48" s="4">
         <v>44012</v>
       </c>
       <c r="H48" s="1">
@@ -7374,17 +7371,17 @@
       <c r="AJ48" s="1">
         <v>113.51351351351373</v>
       </c>
-      <c r="AK48" s="4">
-        <v>11.904761904762076</v>
-      </c>
-      <c r="AL48" s="12">
+      <c r="AK48" s="1">
+        <v>13.513513513513733</v>
+      </c>
+      <c r="AL48" s="11">
         <v>178</v>
       </c>
-      <c r="AM48" s="12">
+      <c r="AM48" s="11">
         <v>190</v>
       </c>
-      <c r="AN48" s="11"/>
-      <c r="AO48" s="11"/>
+      <c r="AN48" s="10"/>
+      <c r="AO48" s="10"/>
       <c r="AP48" s="2">
         <f t="shared" si="6"/>
         <v>184</v>
@@ -7403,13 +7400,13 @@
       <c r="D49" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E49" s="18" t="s">
+      <c r="E49" s="17" t="s">
         <v>141</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G49" s="5">
+      <c r="G49" s="4">
         <v>44012</v>
       </c>
       <c r="H49" s="1">
@@ -7506,19 +7503,19 @@
       <c r="AJ49" s="1">
         <v>3.8955823293172855</v>
       </c>
-      <c r="AK49" s="4">
-        <v>51.546391752576916</v>
+      <c r="AK49" s="1">
+        <v>2.0080321285140492</v>
       </c>
       <c r="AL49" s="2">
         <v>1680</v>
       </c>
-      <c r="AM49" s="13">
+      <c r="AM49" s="12">
         <v>0</v>
       </c>
       <c r="AN49" s="2">
         <v>1770</v>
       </c>
-      <c r="AO49" s="13">
+      <c r="AO49" s="12">
         <v>0</v>
       </c>
       <c r="AP49" s="2">
@@ -7545,7 +7542,7 @@
       <c r="F50" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G50" s="5">
+      <c r="G50" s="4">
         <v>43899</v>
       </c>
       <c r="H50" s="2">
@@ -7642,8 +7639,8 @@
       <c r="AJ50" s="1">
         <v>2.0030816640986258</v>
       </c>
-      <c r="AK50" s="4">
-        <v>61.53846153846122</v>
+      <c r="AK50" s="1">
+        <v>1.2326656394453017</v>
       </c>
       <c r="AL50" s="2">
         <v>1200</v>
@@ -7651,10 +7648,10 @@
       <c r="AM50" s="2">
         <v>1800</v>
       </c>
-      <c r="AN50" s="13">
+      <c r="AN50" s="12">
         <v>0</v>
       </c>
-      <c r="AO50" s="13">
+      <c r="AO50" s="12">
         <v>0</v>
       </c>
       <c r="AP50" s="2">
@@ -7681,7 +7678,7 @@
       <c r="F51" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G51" s="5">
+      <c r="G51" s="4">
         <v>43899</v>
       </c>
       <c r="H51" s="2">
@@ -7778,8 +7775,8 @@
       <c r="AJ51" s="1">
         <v>0.76569678407351782</v>
       </c>
-      <c r="AK51" s="4">
-        <v>39.999999999998579</v>
+      <c r="AK51" s="1">
+        <v>0.30627871362939624</v>
       </c>
       <c r="AL51" s="2">
         <v>1800</v>
@@ -7790,7 +7787,7 @@
       <c r="AN51" s="2">
         <v>1000</v>
       </c>
-      <c r="AO51" s="13">
+      <c r="AO51" s="12">
         <v>0</v>
       </c>
       <c r="AP51" s="2">
@@ -7817,7 +7814,7 @@
       <c r="F52" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G52" s="5">
+      <c r="G52" s="4">
         <v>43899</v>
       </c>
       <c r="H52" s="2">
@@ -7914,17 +7911,17 @@
       <c r="AJ52" s="1">
         <v>18.283963227783435</v>
       </c>
-      <c r="AK52" s="4">
-        <v>27.653631284916287</v>
-      </c>
-      <c r="AL52" s="12">
+      <c r="AK52" s="1">
+        <v>5.0561797752809099</v>
+      </c>
+      <c r="AL52" s="11">
         <v>24</v>
       </c>
-      <c r="AM52" s="12">
+      <c r="AM52" s="11">
         <v>35</v>
       </c>
-      <c r="AN52" s="11"/>
-      <c r="AO52" s="11"/>
+      <c r="AN52" s="10"/>
+      <c r="AO52" s="10"/>
       <c r="AP52" s="2">
         <f t="shared" si="6"/>
         <v>29.5</v>
@@ -7949,7 +7946,7 @@
       <c r="F53" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G53" s="5">
+      <c r="G53" s="4">
         <v>43899</v>
       </c>
       <c r="H53" s="2">
@@ -8046,8 +8043,8 @@
       <c r="AJ53" s="1">
         <v>3.0330330330330324</v>
       </c>
-      <c r="AK53" s="4">
-        <v>60.396039603960347</v>
+      <c r="AK53" s="1">
+        <v>1.8318318318318298</v>
       </c>
       <c r="AL53" s="2">
         <v>1320</v>
@@ -8058,7 +8055,7 @@
       <c r="AN53" s="2">
         <v>1000</v>
       </c>
-      <c r="AO53" s="14"/>
+      <c r="AO53" s="13"/>
       <c r="AP53" s="2">
         <f t="shared" si="6"/>
         <v>1406.6666666666667</v>
@@ -8077,13 +8074,13 @@
       <c r="D54" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E54" s="17" t="s">
+      <c r="E54" s="16" t="s">
         <v>138</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G54" s="5">
+      <c r="G54" s="4">
         <v>43906</v>
       </c>
       <c r="H54" s="2">
@@ -8180,8 +8177,8 @@
       <c r="AJ54" s="1">
         <v>0.71684587813624889</v>
       </c>
-      <c r="AK54" s="4">
-        <v>49.999999999995559</v>
+      <c r="AK54" s="1">
+        <v>0.35842293906809258</v>
       </c>
       <c r="AL54" s="2">
         <v>1000</v>
@@ -8213,13 +8210,13 @@
       <c r="D55" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E55" s="18" t="s">
+      <c r="E55" s="17" t="s">
         <v>139</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G55" s="5">
+      <c r="G55" s="4">
         <v>43906</v>
       </c>
       <c r="H55" s="2">
@@ -8316,8 +8313,8 @@
       <c r="AJ55" s="1">
         <v>0.70422535211266135</v>
       </c>
-      <c r="AK55" s="4">
-        <v>50</v>
+      <c r="AK55" s="1">
+        <v>0.35211267605633068</v>
       </c>
       <c r="AL55" s="2">
         <v>350</v>
@@ -8349,13 +8346,13 @@
       <c r="D56" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E56" s="18" t="s">
+      <c r="E56" s="17" t="s">
         <v>140</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G56" s="5">
+      <c r="G56" s="4">
         <v>43906</v>
       </c>
       <c r="H56" s="2">
@@ -8452,17 +8449,17 @@
       <c r="AJ56" s="1">
         <v>28.949771689497716</v>
       </c>
-      <c r="AK56" s="4">
-        <v>5.3627760252367001</v>
-      </c>
-      <c r="AL56" s="12">
+      <c r="AK56" s="1">
+        <v>1.5525114155251449</v>
+      </c>
+      <c r="AL56" s="11">
         <v>3</v>
       </c>
-      <c r="AM56" s="12">
+      <c r="AM56" s="11">
         <v>2</v>
       </c>
-      <c r="AN56" s="11"/>
-      <c r="AO56" s="11"/>
+      <c r="AN56" s="10"/>
+      <c r="AO56" s="10"/>
       <c r="AP56" s="2">
         <f t="shared" si="6"/>
         <v>2.5</v>
@@ -8481,13 +8478,13 @@
       <c r="D57" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E57" s="18" t="s">
+      <c r="E57" s="17" t="s">
         <v>141</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G57" s="5">
+      <c r="G57" s="4">
         <v>43906</v>
       </c>
       <c r="H57" s="2">
@@ -8584,8 +8581,8 @@
       <c r="AJ57" s="1">
         <v>2.8514056224899846</v>
       </c>
-      <c r="AK57" s="4">
-        <v>43.66197183098636</v>
+      <c r="AK57" s="1">
+        <v>1.2449799196787383</v>
       </c>
       <c r="AL57" s="2">
         <v>190</v>
@@ -8623,7 +8620,7 @@
       <c r="F58" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G58" s="5">
+      <c r="G58" s="4">
         <v>43977</v>
       </c>
       <c r="H58" s="2">
@@ -8720,8 +8717,8 @@
       <c r="AJ58" s="1">
         <v>0.99410005657479994</v>
       </c>
-      <c r="AK58" s="4">
-        <v>55.284552845528324</v>
+      <c r="AK58" s="1">
+        <v>0.54958377111452217</v>
       </c>
       <c r="AL58" s="2">
         <v>2000</v>
@@ -8759,7 +8756,7 @@
       <c r="F59" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G59" s="5">
+      <c r="G59" s="4">
         <v>43977</v>
       </c>
       <c r="H59" s="2">
@@ -8856,8 +8853,8 @@
       <c r="AJ59" s="1">
         <v>0.68438643959891765</v>
       </c>
-      <c r="AK59" s="4">
-        <v>45.736434108527085</v>
+      <c r="AK59" s="1">
+        <v>0.31301395299485352</v>
       </c>
       <c r="AL59" s="2">
         <v>600</v>
@@ -8895,7 +8892,7 @@
       <c r="F60" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G60" s="5">
+      <c r="G60" s="4">
         <v>43977</v>
       </c>
       <c r="H60" s="2">
@@ -8992,17 +8989,17 @@
       <c r="AJ60" s="1">
         <v>21.259842519685041</v>
       </c>
-      <c r="AK60" s="4">
-        <v>70.370370370370352</v>
-      </c>
-      <c r="AL60" s="12">
+      <c r="AK60" s="1">
+        <v>14.960629921259841</v>
+      </c>
+      <c r="AL60" s="11">
         <v>104</v>
       </c>
-      <c r="AM60" s="12">
+      <c r="AM60" s="11">
         <v>100</v>
       </c>
-      <c r="AN60" s="11"/>
-      <c r="AO60" s="11"/>
+      <c r="AN60" s="10"/>
+      <c r="AO60" s="10"/>
       <c r="AP60" s="2">
         <f t="shared" si="6"/>
         <v>102</v>
@@ -9027,7 +9024,7 @@
       <c r="F61" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G61" s="5">
+      <c r="G61" s="4">
         <v>43977</v>
       </c>
       <c r="H61" s="2">
@@ -9124,8 +9121,8 @@
       <c r="AJ61" s="1">
         <v>0.83012981224580751</v>
       </c>
-      <c r="AK61" s="4">
-        <v>60.402684563758278</v>
+      <c r="AK61" s="1">
+        <v>0.50142069196055394</v>
       </c>
       <c r="AL61" s="2">
         <v>2000</v>
@@ -9136,7 +9133,7 @@
       <c r="AN61" s="2">
         <v>14000</v>
       </c>
-      <c r="AO61" s="14"/>
+      <c r="AO61" s="13"/>
       <c r="AP61" s="2">
         <f t="shared" si="6"/>
         <v>8266.6666666666661</v>
@@ -9155,13 +9152,13 @@
       <c r="D62" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E62" s="17" t="s">
+      <c r="E62" s="16" t="s">
         <v>138</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G62" s="5">
+      <c r="G62" s="4">
         <v>43979</v>
       </c>
       <c r="H62" s="2">
@@ -9258,8 +9255,8 @@
       <c r="AJ62" s="1">
         <v>0.44362505041193862</v>
       </c>
-      <c r="AK62" s="4">
-        <v>51.948051948051877</v>
+      <c r="AK62" s="1">
+        <v>0.23045457164256519</v>
       </c>
       <c r="AL62" s="2">
         <v>600</v>
@@ -9291,13 +9288,13 @@
       <c r="D63" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E63" s="18" t="s">
+      <c r="E63" s="17" t="s">
         <v>139</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G63" s="5">
+      <c r="G63" s="4">
         <v>43979</v>
       </c>
       <c r="H63" s="2">
@@ -9394,8 +9391,8 @@
       <c r="AJ63" s="1">
         <v>0.77253218884120234</v>
       </c>
-      <c r="AK63" s="4">
-        <v>35.555555555555557</v>
+      <c r="AK63" s="1">
+        <v>0.27467811158798305</v>
       </c>
       <c r="AL63" s="2">
         <v>600</v>
@@ -9427,13 +9424,13 @@
       <c r="D64" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E64" s="18" t="s">
+      <c r="E64" s="17" t="s">
         <v>140</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G64" s="5">
+      <c r="G64" s="4">
         <v>43979</v>
       </c>
       <c r="H64" s="2">
@@ -9530,17 +9527,17 @@
       <c r="AJ64" s="1">
         <v>15.783540022547914</v>
       </c>
-      <c r="AK64" s="4">
-        <v>69.642857142857167</v>
-      </c>
-      <c r="AL64" s="12">
+      <c r="AK64" s="1">
+        <v>10.99210822998873</v>
+      </c>
+      <c r="AL64" s="11">
         <v>36</v>
       </c>
-      <c r="AM64" s="12">
+      <c r="AM64" s="11">
         <v>45</v>
       </c>
-      <c r="AN64" s="11"/>
-      <c r="AO64" s="11"/>
+      <c r="AN64" s="10"/>
+      <c r="AO64" s="10"/>
       <c r="AP64" s="2">
         <f t="shared" si="6"/>
         <v>40.5</v>
@@ -9559,13 +9556,13 @@
       <c r="D65" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E65" s="18" t="s">
+      <c r="E65" s="17" t="s">
         <v>141</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G65" s="5">
+      <c r="G65" s="4">
         <v>43979</v>
       </c>
       <c r="H65" s="2">
@@ -9662,8 +9659,8 @@
       <c r="AJ65" s="1">
         <v>1.6990291262136026</v>
       </c>
-      <c r="AK65" s="4">
-        <v>14.285714285714739</v>
+      <c r="AK65" s="1">
+        <v>0.24271844660195094</v>
       </c>
       <c r="AL65" s="2">
         <v>600</v>
@@ -9701,7 +9698,7 @@
       <c r="F66" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G66" s="5">
+      <c r="G66" s="4">
         <v>43983</v>
       </c>
       <c r="H66" s="2">
@@ -9798,8 +9795,8 @@
       <c r="AJ66" s="1">
         <v>1.1226252158894636</v>
       </c>
-      <c r="AK66" s="4">
-        <v>53.846153846153769</v>
+      <c r="AK66" s="1">
+        <v>0.60449050086355649</v>
       </c>
       <c r="AL66" s="2">
         <v>1400</v>
@@ -9837,7 +9834,7 @@
       <c r="F67" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G67" s="5">
+      <c r="G67" s="4">
         <v>43983</v>
       </c>
       <c r="H67" s="2">
@@ -9934,8 +9931,8 @@
       <c r="AJ67" s="1">
         <v>0.64364207221350134</v>
       </c>
-      <c r="AK67" s="4">
-        <v>36.585365853658537</v>
+      <c r="AK67" s="1">
+        <v>0.23547880690737855</v>
       </c>
       <c r="AL67" s="2">
         <v>940</v>
@@ -9973,7 +9970,7 @@
       <c r="F68" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G68" s="5">
+      <c r="G68" s="4">
         <v>43983</v>
       </c>
       <c r="H68" s="2">
@@ -10070,17 +10067,17 @@
       <c r="AJ68" s="1">
         <v>13.443830570902396</v>
       </c>
-      <c r="AK68" s="4">
-        <v>68.493150684931507</v>
-      </c>
-      <c r="AL68" s="12">
+      <c r="AK68" s="1">
+        <v>9.2081031307550649</v>
+      </c>
+      <c r="AL68" s="11">
         <v>100</v>
       </c>
-      <c r="AM68" s="12">
+      <c r="AM68" s="11">
         <v>120</v>
       </c>
-      <c r="AN68" s="11"/>
-      <c r="AO68" s="11"/>
+      <c r="AN68" s="10"/>
+      <c r="AO68" s="10"/>
       <c r="AP68" s="2">
         <f t="shared" si="15"/>
         <v>110</v>
@@ -10105,7 +10102,7 @@
       <c r="F69" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G69" s="5">
+      <c r="G69" s="4">
         <v>43983</v>
       </c>
       <c r="H69" s="2">
@@ -10202,8 +10199,8 @@
       <c r="AJ69" s="1">
         <v>0.92502001245219134</v>
       </c>
-      <c r="AK69" s="4">
-        <v>57.692307692307601</v>
+      <c r="AK69" s="1">
+        <v>0.53366539179934025</v>
       </c>
       <c r="AL69" s="2">
         <v>1000</v>
@@ -10235,13 +10232,13 @@
       <c r="D70" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E70" s="17" t="s">
+      <c r="E70" s="16" t="s">
         <v>138</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G70" s="5">
+      <c r="G70" s="4">
         <v>43987</v>
       </c>
       <c r="H70" s="2">
@@ -10338,8 +10335,8 @@
       <c r="AJ70" s="1">
         <v>1.4489209512746843</v>
       </c>
-      <c r="AK70" s="4">
-        <v>12.658227848101273</v>
+      <c r="AK70" s="1">
+        <v>0.18340771535122596</v>
       </c>
       <c r="AL70" s="2">
         <v>1320</v>
@@ -10371,13 +10368,13 @@
       <c r="D71" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E71" s="18" t="s">
+      <c r="E71" s="17" t="s">
         <v>139</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G71" s="5">
+      <c r="G71" s="4">
         <v>43987</v>
       </c>
       <c r="H71" s="2">
@@ -10474,8 +10471,8 @@
       <c r="AJ71" s="1">
         <v>2.0270270270270272</v>
       </c>
-      <c r="AK71" s="4">
-        <v>16.666666666666682</v>
+      <c r="AK71" s="1">
+        <v>0.33783783783783816</v>
       </c>
       <c r="AL71" s="2">
         <v>400</v>
@@ -10507,13 +10504,13 @@
       <c r="D72" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E72" s="18" t="s">
+      <c r="E72" s="17" t="s">
         <v>140</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G72" s="5">
+      <c r="G72" s="4">
         <v>43987</v>
       </c>
       <c r="H72" s="2">
@@ -10610,17 +10607,17 @@
       <c r="AJ72" s="1">
         <v>10.939167556029879</v>
       </c>
-      <c r="AK72" s="4">
-        <v>15.121951219512159</v>
-      </c>
-      <c r="AL72" s="12">
+      <c r="AK72" s="1">
+        <v>1.6542155816435389</v>
+      </c>
+      <c r="AL72" s="11">
         <v>140</v>
       </c>
-      <c r="AM72" s="12">
+      <c r="AM72" s="11">
         <v>164</v>
       </c>
-      <c r="AN72" s="11"/>
-      <c r="AO72" s="11"/>
+      <c r="AN72" s="10"/>
+      <c r="AO72" s="10"/>
       <c r="AP72" s="2">
         <f t="shared" si="15"/>
         <v>152</v>
@@ -10639,13 +10636,13 @@
       <c r="D73" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E73" s="18" t="s">
+      <c r="E73" s="17" t="s">
         <v>141</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G73" s="5">
+      <c r="G73" s="4">
         <v>43987</v>
       </c>
       <c r="H73" s="2">
@@ -10742,8 +10739,8 @@
       <c r="AJ73" s="1">
         <v>13.834951456310682</v>
       </c>
-      <c r="AK73" s="4">
-        <v>18.128654970760181</v>
+      <c r="AK73" s="1">
+        <v>2.5080906148867244</v>
       </c>
       <c r="AL73" s="2">
         <v>300</v>
@@ -10781,7 +10778,7 @@
       <c r="F74" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G74" s="5">
+      <c r="G74" s="4">
         <v>43991</v>
       </c>
       <c r="H74" s="2">
@@ -10878,8 +10875,8 @@
       <c r="AJ74" s="1">
         <v>2.1052631578946936</v>
       </c>
-      <c r="AK74" s="4">
-        <v>50</v>
+      <c r="AK74" s="1">
+        <v>1.0526315789473468</v>
       </c>
       <c r="AL74" s="2">
         <v>2000</v>
@@ -10917,7 +10914,7 @@
       <c r="F75" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G75" s="5">
+      <c r="G75" s="4">
         <v>43991</v>
       </c>
       <c r="H75" s="2">
@@ -11014,8 +11011,8 @@
       <c r="AJ75" s="1">
         <v>15.189873417721531</v>
       </c>
-      <c r="AK75" s="4">
-        <v>8.3333333333331474</v>
+      <c r="AK75" s="1">
+        <v>1.2658227848100994</v>
       </c>
       <c r="AL75" s="2">
         <v>960</v>
@@ -11053,7 +11050,7 @@
       <c r="F76" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G76" s="5">
+      <c r="G76" s="4">
         <v>43991</v>
       </c>
       <c r="H76" s="2">
@@ -11150,17 +11147,17 @@
       <c r="AJ76" s="1">
         <v>59.624413145539833</v>
       </c>
-      <c r="AK76" s="4">
-        <v>7.874015748031324</v>
-      </c>
-      <c r="AL76" s="12">
+      <c r="AK76" s="1">
+        <v>4.6948356807510656</v>
+      </c>
+      <c r="AL76" s="11">
         <v>200</v>
       </c>
-      <c r="AM76" s="12">
+      <c r="AM76" s="11">
         <v>200</v>
       </c>
-      <c r="AN76" s="11"/>
-      <c r="AO76" s="11"/>
+      <c r="AN76" s="10"/>
+      <c r="AO76" s="10"/>
       <c r="AP76" s="2">
         <f t="shared" si="15"/>
         <v>200</v>
@@ -11185,7 +11182,7 @@
       <c r="F77" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G77" s="5">
+      <c r="G77" s="4">
         <v>43991</v>
       </c>
       <c r="H77" s="2">
@@ -11282,8 +11279,8 @@
       <c r="AJ77" s="1">
         <v>21.94570135746595</v>
       </c>
-      <c r="AK77" s="4">
-        <v>47.422680412370724</v>
+      <c r="AK77" s="1">
+        <v>10.407239819004381</v>
       </c>
       <c r="AL77" s="2">
         <v>1200</v>
@@ -11315,13 +11312,13 @@
       <c r="D78" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E78" s="17" t="s">
+      <c r="E78" s="16" t="s">
         <v>138</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G78" s="5">
+      <c r="G78" s="4">
         <v>43994</v>
       </c>
       <c r="H78" s="2">
@@ -11418,8 +11415,8 @@
       <c r="AJ78" s="1">
         <v>0.97008892481810738</v>
       </c>
-      <c r="AK78" s="4">
-        <v>15.000000000000027</v>
+      <c r="AK78" s="1">
+        <v>0.14551333872271635</v>
       </c>
       <c r="AL78" s="2">
         <v>1200</v>
@@ -11451,13 +11448,13 @@
       <c r="D79" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E79" s="18" t="s">
+      <c r="E79" s="17" t="s">
         <v>139</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G79" s="5">
+      <c r="G79" s="4">
         <v>43994</v>
       </c>
       <c r="H79" s="2">
@@ -11554,8 +11551,8 @@
       <c r="AJ79" s="1">
         <v>0.6000106196569851</v>
       </c>
-      <c r="AK79" s="4">
-        <v>26.548672566371511</v>
+      <c r="AK79" s="1">
+        <v>0.15929485477618971</v>
       </c>
       <c r="AL79" s="2">
         <v>360</v>
@@ -11587,13 +11584,13 @@
       <c r="D80" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E80" s="18" t="s">
+      <c r="E80" s="17" t="s">
         <v>140</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G80" s="5">
+      <c r="G80" s="4">
         <v>43994</v>
       </c>
       <c r="H80" s="2">
@@ -11690,17 +11687,17 @@
       <c r="AJ80" s="1">
         <v>21.259842519685041</v>
       </c>
-      <c r="AK80" s="4">
-        <v>22.259259259259274</v>
-      </c>
-      <c r="AL80" s="12">
+      <c r="AK80" s="1">
+        <v>4.7322834645669323</v>
+      </c>
+      <c r="AL80" s="11">
         <v>144</v>
       </c>
-      <c r="AM80" s="12">
+      <c r="AM80" s="11">
         <v>165</v>
       </c>
-      <c r="AN80" s="11"/>
-      <c r="AO80" s="11"/>
+      <c r="AN80" s="10"/>
+      <c r="AO80" s="10"/>
       <c r="AP80" s="2">
         <f t="shared" si="15"/>
         <v>154.5</v>
@@ -11719,13 +11716,13 @@
       <c r="D81" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E81" s="18" t="s">
+      <c r="E81" s="17" t="s">
         <v>141</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G81" s="5">
+      <c r="G81" s="4">
         <v>43994</v>
       </c>
       <c r="H81" s="2">
@@ -11822,8 +11819,8 @@
       <c r="AJ81" s="1">
         <v>0.8190783975037611</v>
       </c>
-      <c r="AK81" s="4">
-        <v>21.088435374149601</v>
+      <c r="AK81" s="1">
+        <v>0.17273081852120081</v>
       </c>
       <c r="AL81" s="2">
         <v>500</v>
@@ -11861,7 +11858,7 @@
       <c r="F82" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G82" s="5">
+      <c r="G82" s="4">
         <v>43998</v>
       </c>
       <c r="H82" s="2">
@@ -11958,8 +11955,8 @@
       <c r="AJ82" s="1">
         <v>1.2924071082390953</v>
       </c>
-      <c r="AK82" s="4">
-        <v>34.408602150537675</v>
+      <c r="AK82" s="1">
+        <v>0.44469922003925916</v>
       </c>
       <c r="AL82" s="2">
         <v>510</v>
@@ -11997,7 +11994,7 @@
       <c r="F83" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G83" s="5">
+      <c r="G83" s="4">
         <v>43998</v>
       </c>
       <c r="H83" s="2">
@@ -12094,8 +12091,8 @@
       <c r="AJ83" s="1">
         <v>0.79544568353739376</v>
       </c>
-      <c r="AK83" s="4">
-        <v>23.529411764705912</v>
+      <c r="AK83" s="1">
+        <v>0.18716369024409288</v>
       </c>
       <c r="AL83" s="2">
         <v>800</v>
@@ -12133,7 +12130,7 @@
       <c r="F84" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G84" s="5">
+      <c r="G84" s="4">
         <v>43998</v>
       </c>
       <c r="H84" s="2">
@@ -12230,17 +12227,17 @@
       <c r="AJ84" s="1">
         <v>18.464309840126099</v>
       </c>
-      <c r="AK84" s="4">
-        <v>16.000000000000014</v>
-      </c>
-      <c r="AL84" s="12">
+      <c r="AK84" s="1">
+        <v>2.9542895744201787</v>
+      </c>
+      <c r="AL84" s="11">
         <v>168</v>
       </c>
-      <c r="AM84" s="12">
+      <c r="AM84" s="11">
         <v>180</v>
       </c>
-      <c r="AN84" s="11"/>
-      <c r="AO84" s="11"/>
+      <c r="AN84" s="10"/>
+      <c r="AO84" s="10"/>
       <c r="AP84" s="2">
         <f t="shared" si="15"/>
         <v>174</v>
@@ -12265,7 +12262,7 @@
       <c r="F85" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G85" s="5">
+      <c r="G85" s="4">
         <v>43998</v>
       </c>
       <c r="H85" s="2">
@@ -12362,8 +12359,8 @@
       <c r="AJ85" s="1">
         <v>1.0034044078122202</v>
       </c>
-      <c r="AK85" s="4">
-        <v>39.473684210526372</v>
+      <c r="AK85" s="1">
+        <v>0.39608068729429802</v>
       </c>
       <c r="AL85" s="2">
         <v>390</v>
@@ -12395,13 +12392,13 @@
       <c r="D86" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E86" s="17" t="s">
+      <c r="E86" s="16" t="s">
         <v>138</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G86" s="5">
+      <c r="G86" s="4">
         <v>44000</v>
       </c>
       <c r="H86" s="2">
@@ -12498,8 +12495,8 @@
       <c r="AJ86" s="1">
         <v>2.4233128834355475</v>
       </c>
-      <c r="AK86" s="4">
-        <v>36.708860759494101</v>
+      <c r="AK86" s="1">
+        <v>0.88957055214723668</v>
       </c>
       <c r="AL86" s="2">
         <v>1280</v>
@@ -12531,13 +12528,13 @@
       <c r="D87" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E87" s="18" t="s">
+      <c r="E87" s="17" t="s">
         <v>139</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G87" s="5">
+      <c r="G87" s="4">
         <v>44000</v>
       </c>
       <c r="H87" s="2">
@@ -12634,8 +12631,8 @@
       <c r="AJ87" s="1">
         <v>2.7946537059538161</v>
       </c>
-      <c r="AK87" s="4">
-        <v>32.608695652173346</v>
+      <c r="AK87" s="1">
+        <v>0.91130012150666329</v>
       </c>
       <c r="AL87" s="2">
         <v>1600</v>
@@ -12667,13 +12664,13 @@
       <c r="D88" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E88" s="18" t="s">
+      <c r="E88" s="17" t="s">
         <v>140</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G88" s="5">
+      <c r="G88" s="4">
         <v>44000</v>
       </c>
       <c r="H88" s="2">
@@ -12770,17 +12767,17 @@
       <c r="AJ88" s="1">
         <v>11.205073995771652</v>
       </c>
-      <c r="AK88" s="4">
-        <v>75.471698113207708</v>
-      </c>
-      <c r="AL88" s="12">
+      <c r="AK88" s="1">
+        <v>8.4566596194503205</v>
+      </c>
+      <c r="AL88" s="11">
         <v>240</v>
       </c>
-      <c r="AM88" s="12">
+      <c r="AM88" s="11">
         <v>200</v>
       </c>
-      <c r="AN88" s="11"/>
-      <c r="AO88" s="11"/>
+      <c r="AN88" s="10"/>
+      <c r="AO88" s="10"/>
       <c r="AP88" s="2">
         <f t="shared" si="15"/>
         <v>220</v>
@@ -12799,13 +12796,13 @@
       <c r="D89" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E89" s="18" t="s">
+      <c r="E89" s="17" t="s">
         <v>141</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G89" s="5">
+      <c r="G89" s="4">
         <v>44000</v>
       </c>
       <c r="H89" s="2">
@@ -12902,8 +12899,8 @@
       <c r="AJ89" s="1">
         <v>1.37825421133231</v>
       </c>
-      <c r="AK89" s="4">
-        <v>44.444444444443562</v>
+      <c r="AK89" s="1">
+        <v>0.61255742725879225</v>
       </c>
       <c r="AL89" s="2">
         <v>1200</v>
@@ -12941,7 +12938,7 @@
       <c r="F90" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G90" s="5">
+      <c r="G90" s="4">
         <v>44011</v>
       </c>
       <c r="H90" s="2">
@@ -13035,7 +13032,7 @@
         <f t="shared" si="14"/>
         <v>1.2666666666666666</v>
       </c>
-      <c r="AJ90" s="6"/>
+      <c r="AJ90" s="5"/>
       <c r="AK90" s="6"/>
       <c r="AL90" s="2">
         <v>1800</v>
@@ -13073,7 +13070,7 @@
       <c r="F91" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G91" s="5">
+      <c r="G91" s="4">
         <v>44011</v>
       </c>
       <c r="H91" s="2">
@@ -13167,7 +13164,7 @@
         <f t="shared" si="14"/>
         <v>1.3999999999999997</v>
       </c>
-      <c r="AJ91" s="6"/>
+      <c r="AJ91" s="5"/>
       <c r="AK91" s="6"/>
       <c r="AL91" s="2">
         <v>1280</v>
@@ -13205,7 +13202,7 @@
       <c r="F92" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G92" s="5">
+      <c r="G92" s="4">
         <v>44011</v>
       </c>
       <c r="H92" s="2">
@@ -13299,16 +13296,16 @@
         <f t="shared" si="14"/>
         <v>1.3666666666666665</v>
       </c>
-      <c r="AJ92" s="6"/>
+      <c r="AJ92" s="5"/>
       <c r="AK92" s="6"/>
-      <c r="AL92" s="12">
+      <c r="AL92" s="11">
         <v>104</v>
       </c>
-      <c r="AM92" s="12">
+      <c r="AM92" s="11">
         <v>112</v>
       </c>
-      <c r="AN92" s="11"/>
-      <c r="AO92" s="11"/>
+      <c r="AN92" s="10"/>
+      <c r="AO92" s="10"/>
       <c r="AP92" s="2">
         <f t="shared" si="15"/>
         <v>108</v>
@@ -13333,7 +13330,7 @@
       <c r="F93" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G93" s="5">
+      <c r="G93" s="4">
         <v>44011</v>
       </c>
       <c r="H93" s="2">
@@ -13427,7 +13424,7 @@
         <f t="shared" si="14"/>
         <v>1.2666666666666666</v>
       </c>
-      <c r="AJ93" s="6"/>
+      <c r="AJ93" s="5"/>
       <c r="AK93" s="6"/>
       <c r="AL93" s="2">
         <v>1240</v>
@@ -13438,7 +13435,7 @@
       <c r="AN93" s="2">
         <v>9000</v>
       </c>
-      <c r="AO93" s="14"/>
+      <c r="AO93" s="13"/>
       <c r="AP93" s="2">
         <f t="shared" si="15"/>
         <v>4613.333333333333</v>
@@ -13457,13 +13454,13 @@
       <c r="D94" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E94" s="17" t="s">
+      <c r="E94" s="16" t="s">
         <v>138</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G94" s="5">
+      <c r="G94" s="4">
         <v>44012</v>
       </c>
       <c r="H94" s="2">
@@ -13560,8 +13557,8 @@
       <c r="AJ94" s="1">
         <v>1.8433179723501911</v>
       </c>
-      <c r="AK94" s="4">
-        <v>25</v>
+      <c r="AK94" s="1">
+        <v>0.46082949308754778</v>
       </c>
       <c r="AL94" s="2">
         <v>1060</v>
@@ -13593,13 +13590,13 @@
       <c r="D95" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E95" s="18" t="s">
+      <c r="E95" s="17" t="s">
         <v>139</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G95" s="5">
+      <c r="G95" s="4">
         <v>44012</v>
       </c>
       <c r="H95" s="2">
@@ -13696,8 +13693,8 @@
       <c r="AJ95" s="1">
         <v>1.8615040953090027</v>
       </c>
-      <c r="AK95" s="4">
-        <v>60.000000000000711</v>
+      <c r="AK95" s="1">
+        <v>1.1169024571854149</v>
       </c>
       <c r="AL95" s="2">
         <v>2240</v>
@@ -13729,13 +13726,13 @@
       <c r="D96" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E96" s="18" t="s">
+      <c r="E96" s="17" t="s">
         <v>140</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G96" s="5">
+      <c r="G96" s="4">
         <v>44012</v>
       </c>
       <c r="H96" s="2">
@@ -13832,17 +13829,17 @@
       <c r="AJ96" s="1">
         <v>15.182357930449552</v>
       </c>
-      <c r="AK96" s="4">
-        <v>14.525139664804337</v>
-      </c>
-      <c r="AL96" s="12">
+      <c r="AK96" s="1">
+        <v>2.205258693808295</v>
+      </c>
+      <c r="AL96" s="11">
         <v>60</v>
       </c>
-      <c r="AM96" s="12">
+      <c r="AM96" s="11">
         <v>50</v>
       </c>
-      <c r="AN96" s="11"/>
-      <c r="AO96" s="11"/>
+      <c r="AN96" s="10"/>
+      <c r="AO96" s="10"/>
       <c r="AP96" s="2">
         <f t="shared" si="15"/>
         <v>55</v>
@@ -13861,13 +13858,13 @@
       <c r="D97" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E97" s="18" t="s">
+      <c r="E97" s="17" t="s">
         <v>141</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="G97" s="5">
+      <c r="G97" s="4">
         <v>44012</v>
       </c>
       <c r="H97" s="2">
@@ -13964,8 +13961,8 @@
       <c r="AJ97" s="1">
         <v>5.7843996494303465</v>
       </c>
-      <c r="AK97" s="4">
-        <v>22.727272727272819</v>
+      <c r="AK97" s="1">
+        <v>1.3146362839614476</v>
       </c>
       <c r="AL97" s="2">
         <v>1000</v>

</xml_diff>